<commit_message>
added tri6, quad8, and quad9 elements to mesh generation. updated seep.py to work with tri6 elements.
</commit_message>
<xml_diff>
--- a/inputs/slope/input_template_lface5.xlsx
+++ b/inputs/slope/input_template_lface5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/CursorProjects/xslope/inputs/slope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2616612-3379-384D-B01E-B8195039E7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513A1566-8232-BC4B-AB3F-541A784F41AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="880" windowWidth="29340" windowHeight="17300" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="3060" yWindow="880" windowWidth="29340" windowHeight="17300" activeTab="9" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -5649,8 +5649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847CAF5A-5624-4041-9578-842C28E166A5}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5679,7 +5679,7 @@
         <v>111</v>
       </c>
       <c r="C3" s="31">
-        <v>302</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>111</v>
@@ -6400,16 +6400,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6419,7 +6419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>